<commit_message>
TC_10 added with keyword driven API's
</commit_message>
<xml_diff>
--- a/testdata/EmpData.xlsx
+++ b/testdata/EmpData.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9264"/>
+    <workbookView windowWidth="23040" windowHeight="9264" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="KWD" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="6">
   <si>
     <t>EMPNAME</t>
   </si>
@@ -86,6 +87,90 @@
   </si>
   <si>
     <t>{"name":"SCOTT161","salary":"55","age":"73005","id":"2681"}</t>
+  </si>
+  <si>
+    <t>API Call</t>
+  </si>
+  <si>
+    <t>Endpoint</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Status Code</t>
+  </si>
+  <si>
+    <t>Resposne</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>/api/users/2</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>{"data":{"id":2,"email":"janet.weaver@reqres.in","first_name":"Janet","last_name":"Weaver","avatar":"https://s3.amazonaws.com/uifaces/faces/twitter/josephstein/128.jpg"}}</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>/api/users</t>
+  </si>
+  <si>
+    <t>{
+    "name": "morpheus",
+    "job": "leader"
+}</t>
+  </si>
+  <si>
+    <t>{"name":"morpheus","job":"leader","id":"264","createdAt":"2019-08-11T11:11:28.636Z"}</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>{
+    "name": "morpheus",
+    "job": "zion resident"
+}</t>
+  </si>
+  <si>
+    <t>{"name":"morpheus","job":"zion resident","updatedAt":"2019-08-11T11:11:29.147Z"}</t>
+  </si>
+  <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t>{"name":"morpheus","job":"zion resident","updatedAt":"2019-08-11T11:11:29.651Z"}</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>{"name":"morpheus","job":"leader","id":"668","createdAt":"2019-08-11T12:45:22.999Z"}</t>
+  </si>
+  <si>
+    <t>{"name":"morpheus","job":"zion resident","updatedAt":"2019-08-11T12:45:23.587Z"}</t>
+  </si>
+  <si>
+    <t>{"name":"morpheus","job":"zion resident","updatedAt":"2019-08-11T12:45:24.094Z"}</t>
+  </si>
+  <si>
+    <t>{"name":"morpheus","job":"leader","id":"27","createdAt":"2019-08-11T13:10:33.679Z"}</t>
+  </si>
+  <si>
+    <t>{"name":"morpheus","job":"zion resident","updatedAt":"2019-08-11T13:10:34.215Z"}</t>
+  </si>
+  <si>
+    <t>{"name":"morpheus","job":"zion resident","updatedAt":"2019-08-11T13:10:34.757Z"}</t>
   </si>
 </sst>
 </file>
@@ -93,10 +178,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -116,31 +201,32 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -152,6 +238,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -160,48 +260,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -215,16 +290,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,22 +306,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -274,187 +359,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -470,11 +555,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -504,6 +587,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -514,15 +612,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -544,41 +633,37 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -588,141 +673,144 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1046,29 +1134,29 @@
   <sheetPr/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="11.7777777777778" customWidth="1"/>
-    <col min="2" max="2" width="14.6666666666667" customWidth="1"/>
-    <col min="3" max="3" width="14.8888888888889" customWidth="1"/>
-    <col min="4" max="4" width="110.333333333333" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="11.7777777777778" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.6666666666667" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.8888888888889" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="110.333333333333" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="3" customFormat="1" spans="1:4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1210,6 +1298,134 @@
       </c>
       <c r="D11" t="s">
         <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="V5" sqref="F2:V5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="16.2222222222222" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="27.5555555555556" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.2222222222222" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="145.111111111111" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2">
+        <v>200</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" ht="57.6" spans="1:5">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>201</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" ht="57.6" spans="1:5">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4">
+        <v>200</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" ht="57.6" spans="1:5">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6">
+        <v>204</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>